<commit_message>
New features: Generates database. Reads in Hanzi list, Output: anki input file
</commit_message>
<xml_diff>
--- a/hanzi_list.xlsx
+++ b/hanzi_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/voss/Documents/Master Wirtschaftsphysik/3. Semester/Chinese_Vocab_to_Anki/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/voss/Documents/Master Wirtschaftsphysik/3. Semester/anki_vocabulary_automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAEBDA9-6679-0946-BB57-59A3F44F35DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C659E37-852F-A14B-B38B-D1F336F53924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="14280" windowHeight="16660" xr2:uid="{8949169C-D32D-FF47-B3A2-C1A222E5BCFD}"/>
   </bookViews>
@@ -36,12 +36,255 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>Hanzi</t>
   </si>
   <si>
-    <t>貴</t>
+    <t>顧客</t>
+  </si>
+  <si>
+    <t>站</t>
+  </si>
+  <si>
+    <t>野餐</t>
+  </si>
+  <si>
+    <t>超市</t>
+  </si>
+  <si>
+    <t>沙發</t>
+  </si>
+  <si>
+    <t>時鐘</t>
+  </si>
+  <si>
+    <t>白</t>
+  </si>
+  <si>
+    <t>黑</t>
+  </si>
+  <si>
+    <t>紅</t>
+  </si>
+  <si>
+    <t>藍</t>
+  </si>
+  <si>
+    <t>綠</t>
+  </si>
+  <si>
+    <t>黃</t>
+  </si>
+  <si>
+    <t>橙</t>
+  </si>
+  <si>
+    <t>垃圾</t>
+  </si>
+  <si>
+    <t>吃醋</t>
+  </si>
+  <si>
+    <t>羨慕</t>
+  </si>
+  <si>
+    <t>車庫</t>
+  </si>
+  <si>
+    <t>非常</t>
+  </si>
+  <si>
+    <t>北京</t>
+  </si>
+  <si>
+    <t>柏林</t>
+  </si>
+  <si>
+    <t>西班牙</t>
+  </si>
+  <si>
+    <t>比利時</t>
+  </si>
+  <si>
+    <t>巴黎</t>
+  </si>
+  <si>
+    <t>首都</t>
+  </si>
+  <si>
+    <t>地區</t>
+  </si>
+  <si>
+    <t>狀態</t>
+  </si>
+  <si>
+    <t>浴室</t>
+  </si>
+  <si>
+    <t>洗手間</t>
+  </si>
+  <si>
+    <t>數字</t>
+  </si>
+  <si>
+    <t>盆栽</t>
+  </si>
+  <si>
+    <t>花</t>
+  </si>
+  <si>
+    <t>蔥油餅</t>
+  </si>
+  <si>
+    <t>強</t>
+  </si>
+  <si>
+    <t>果子</t>
+  </si>
+  <si>
+    <t>鍋</t>
+  </si>
+  <si>
+    <t>平鍋</t>
+  </si>
+  <si>
+    <t>蔬菜</t>
+  </si>
+  <si>
+    <t>牛肉</t>
+  </si>
+  <si>
+    <t>豬肉</t>
+  </si>
+  <si>
+    <t>羊肉</t>
+  </si>
+  <si>
+    <t>雞</t>
+  </si>
+  <si>
+    <t>衣櫃</t>
+  </si>
+  <si>
+    <t>帶走</t>
+  </si>
+  <si>
+    <t>點菜</t>
+  </si>
+  <si>
+    <t>架子</t>
+  </si>
+  <si>
+    <t>書架</t>
+  </si>
+  <si>
+    <t>一張紙</t>
+  </si>
+  <si>
+    <t>租</t>
+  </si>
+  <si>
+    <t>租金</t>
+  </si>
+  <si>
+    <t>窗戶</t>
+  </si>
+  <si>
+    <t>計程車</t>
+  </si>
+  <si>
+    <t>我自己</t>
+  </si>
+  <si>
+    <t>還沒</t>
+  </si>
+  <si>
+    <t>決定</t>
+  </si>
+  <si>
+    <t>特別的</t>
+  </si>
+  <si>
+    <t>打折</t>
+  </si>
+  <si>
+    <t>信用卡</t>
+  </si>
+  <si>
+    <t>年</t>
+  </si>
+  <si>
+    <t>點</t>
+  </si>
+  <si>
+    <t>有精</t>
+  </si>
+  <si>
+    <t>如果</t>
+  </si>
+  <si>
+    <t>成為</t>
+  </si>
+  <si>
+    <t>巧克力</t>
+  </si>
+  <si>
+    <t>蘋果</t>
+  </si>
+  <si>
+    <t>香蕉</t>
+  </si>
+  <si>
+    <t>草莓</t>
+  </si>
+  <si>
+    <t>梨</t>
+  </si>
+  <si>
+    <t>葡萄</t>
+  </si>
+  <si>
+    <t>檸檬</t>
+  </si>
+  <si>
+    <t>切</t>
+  </si>
+  <si>
+    <t>桃子</t>
+  </si>
+  <si>
+    <t>婚禮</t>
+  </si>
+  <si>
+    <t>結婚</t>
+  </si>
+  <si>
+    <t>生日</t>
+  </si>
+  <si>
+    <t>排球</t>
+  </si>
+  <si>
+    <t>有時候</t>
+  </si>
+  <si>
+    <t>絕不</t>
+  </si>
+  <si>
+    <t>總是</t>
+  </si>
+  <si>
+    <t>游泳</t>
+  </si>
+  <si>
+    <t>游泳池</t>
+  </si>
+  <si>
+    <t>健身房</t>
+  </si>
+  <si>
+    <t>白飯</t>
   </si>
 </sst>
 </file>
@@ -393,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA64E976-6A09-2F43-AFEF-27053D858CB0}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="304" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="241" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -411,6 +654,411 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>